<commit_message>
lots of content (images and text)
</commit_message>
<xml_diff>
--- a/Last Call/Assets/Data/topics.xlsx
+++ b/Last Call/Assets/Data/topics.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="topics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Topic</t>
   </si>
@@ -40,13 +40,106 @@
   </si>
   <si>
     <t>War</t>
+  </si>
+  <si>
+    <t>Nukes</t>
+  </si>
+  <si>
+    <t>Scientists</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Russians</t>
+  </si>
+  <si>
+    <t>Civilians</t>
+  </si>
+  <si>
+    <t>Duty</t>
+  </si>
+  <si>
+    <t>Authority</t>
+  </si>
+  <si>
+    <t>Normality</t>
+  </si>
+  <si>
+    <t>Calamity</t>
+  </si>
+  <si>
+    <t>Justice</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Eroticism</t>
+  </si>
+  <si>
+    <t>Doomsday</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>God</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Indians</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>Childhood</t>
+  </si>
+  <si>
+    <t>Dreamers</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>Civilization</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Confront</t>
+  </si>
+  <si>
+    <t>Forget</t>
+  </si>
+  <si>
+    <t>Destruction</t>
+  </si>
+  <si>
+    <t>Complex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +270,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -523,8 +625,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -846,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,31 +967,244 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>